<commit_message>
Dictating No Recalls on screen
</commit_message>
<xml_diff>
--- a/Data/Input/Ford + Toyota VINs.xlsx
+++ b/Data/Input/Ford + Toyota VINs.xlsx
@@ -6519,7 +6519,7 @@
       <x:selection activeCell="E2" sqref="E2 E2:E16"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="27.557656" defaultRowHeight="15.75" customHeight="1"/>
+  <x:sheetFormatPr defaultColWidth="28.978906" defaultRowHeight="15.75" customHeight="1"/>
   <x:cols>
     <x:col min="1" max="1" width="53.855469" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="5.425781" style="0" hidden="1" customWidth="1"/>
@@ -26586,7 +26586,7 @@
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="27.557656" defaultRowHeight="15.75" customHeight="1"/>
+  <x:sheetFormatPr defaultColWidth="28.978906" defaultRowHeight="15.75" customHeight="1"/>
   <x:cols>
     <x:col min="1" max="1" width="20.425781" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="7.425781" style="0" hidden="1" customWidth="1"/>

</xml_diff>